<commit_message>
Correccion de las funciones fitness, seleccion, crossover, mutation y optimizacion de codigo
</commit_message>
<xml_diff>
--- a/Pruebas.xlsx
+++ b/Pruebas.xlsx
@@ -70,12 +70,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -91,31 +91,33 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -126,14 +128,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -141,92 +174,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,6 +224,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -247,187 +242,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,21 +433,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,17 +469,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -511,15 +480,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,140 +498,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1009,7 +1004,7 @@
   <dimension ref="A2:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.552380952381" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -1027,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:3">
@@ -1035,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>68</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -1043,8 +1038,8 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <f>(80-68)/64</f>
-        <v>0.1875</v>
+        <f>(C3-C2)/64</f>
+        <v>0.015625</v>
       </c>
     </row>
     <row r="5" ht="12.8" customHeight="1" spans="1:4">
@@ -1080,37 +1075,37 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <f>$C$2+(B7*$C$4)</f>
-        <v>85.25</v>
+        <v>4.0625</v>
       </c>
       <c r="D7" s="1">
         <f>(2*SIN(C7))+COS(2*C7)</f>
-        <v>-0.171305832907717</v>
+        <v>-1.86001473215667</v>
       </c>
       <c r="E7" s="3">
         <f>SUM(D7:D12)</f>
-        <v>-0.558299720875876</v>
+        <v>-11.3061521004302</v>
       </c>
       <c r="F7" s="3">
         <f>E7/6</f>
-        <v>-0.0930499534793127</v>
+        <v>-1.88435868340504</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3"/>
       <c r="B8" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <f>$C$2+(B8*$C$4)</f>
-        <v>85.25</v>
+        <v>4.0625</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ref="D7:D42" si="0">(2*SIN(C8))+COS(2*C8)</f>
-        <v>-0.171305832907717</v>
+        <v>-1.86001473215667</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1118,15 +1113,15 @@
     <row r="9" spans="1:6">
       <c r="A9" s="3"/>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <f>$C$2+(B9*$C$4)</f>
-        <v>81.125</v>
+        <v>4.078125</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>-0.614144874016397</v>
+        <v>-1.9087026346534</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1134,15 +1129,15 @@
     <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="1">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <f>$C$2+(B10*$C$4)</f>
-        <v>91.625</v>
+        <v>4.0625</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>-0.483433355665759</v>
+        <v>-1.86001473215667</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1150,15 +1145,15 @@
     <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" s="1">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <f>$C$2+(B11*$C$4)</f>
-        <v>88.4375</v>
+        <v>4.078125</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>1.49603504863811</v>
+        <v>-1.9087026346534</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1166,15 +1161,15 @@
     <row r="12" spans="1:6">
       <c r="A12" s="3"/>
       <c r="B12" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <f>$C$2+(B12*$C$4)</f>
-        <v>81.125</v>
+        <v>4.078125</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.614144874016397</v>
+        <v>-1.9087026346534</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1183,86 +1178,68 @@
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <v>7</v>
-      </c>
       <c r="C13" s="1">
         <f>$C$2+(B13*$C$4)</f>
-        <v>81.3125</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.0187420215754557</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3"/>
-      <c r="B14" s="1">
-        <v>46</v>
-      </c>
       <c r="C14" s="1">
         <f>$C$2+(B14*$C$4)</f>
-        <v>88.625</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>1.47426395750652</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3"/>
-      <c r="B15" s="1">
-        <v>60</v>
-      </c>
       <c r="C15" s="1">
         <f>$C$2+(B15*$C$4)</f>
-        <v>91.25</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>0.672284338936431</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3"/>
-      <c r="B16" s="1">
-        <v>28</v>
-      </c>
       <c r="C16" s="1">
         <f>$C$2+(B16*$C$4)</f>
-        <v>85.25</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>-0.171305832907717</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3"/>
-      <c r="B17" s="1">
-        <v>6</v>
-      </c>
       <c r="C17" s="1">
         <f>$C$2+(B17*$C$4)</f>
-        <v>81.125</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>-0.614144874016397</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3"/>
-      <c r="B18" s="1">
-        <v>30</v>
-      </c>
       <c r="C18" s="1">
         <f>$C$2+(B18*$C$4)</f>
-        <v>85.625</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>-1.47068812765893</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="19" ht="12.8" customHeight="1" spans="1:4">
@@ -1271,66 +1248,66 @@
       </c>
       <c r="C19" s="1">
         <f>$C$2+(B19*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="C20" s="1">
         <f>$C$2+(B20*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3"/>
       <c r="C21" s="1">
         <f>$C$2+(B21*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3"/>
       <c r="C22" s="1">
         <f>$C$2+(B22*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3"/>
       <c r="C23" s="1">
         <f>$C$2+(B23*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3"/>
       <c r="C24" s="1">
         <f>$C$2+(B24*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="25" ht="12.8" customHeight="1" spans="1:4">
@@ -1339,66 +1316,66 @@
       </c>
       <c r="C25" s="1">
         <f>$C$2+(B25*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3"/>
       <c r="C26" s="1">
         <f>$C$2+(B26*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3"/>
       <c r="C27" s="1">
         <f>$C$2+(B27*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3"/>
       <c r="C28" s="1">
         <f>$C$2+(B28*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3"/>
       <c r="C29" s="1">
         <f>$C$2+(B29*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3"/>
       <c r="C30" s="1">
         <f>$C$2+(B30*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="31" ht="12.8" customHeight="1" spans="1:4">
@@ -1407,66 +1384,66 @@
       </c>
       <c r="C31" s="1">
         <f>$C$2+(B31*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3"/>
       <c r="C32" s="1">
         <f>$C$2+(B32*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3"/>
       <c r="C33" s="1">
         <f>$C$2+(B33*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3"/>
       <c r="C34" s="1">
         <f>$C$2+(B34*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3"/>
       <c r="C35" s="1">
         <f>$C$2+(B35*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3"/>
       <c r="C36" s="1">
         <f>$C$2+(B36*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="37" ht="12.8" customHeight="1" spans="1:4">
@@ -1475,66 +1452,66 @@
       </c>
       <c r="C37" s="1">
         <f>$C$2+(B37*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3"/>
       <c r="C38" s="1">
         <f>$C$2+(B38*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3"/>
       <c r="C39" s="1">
         <f>$C$2+(B39*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3"/>
       <c r="C40" s="1">
         <f>$C$2+(B40*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3"/>
       <c r="C41" s="1">
         <f>$C$2+(B41*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3"/>
       <c r="C42" s="1">
         <f>$C$2+(B42*$C$4)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="0"/>
-        <v>-2.96340662064199</v>
+        <v>-1.65910502442447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>